<commit_message>
completed post regression analysis
</commit_message>
<xml_diff>
--- a/regression-results/Report - Regression Runs_Summaries-JI.xlsx
+++ b/regression-results/Report - Regression Runs_Summaries-JI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sifaat\FFC-Forecasting-Study\forecasting-study\regression-results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B7BA03-42DA-4AAD-9694-24565691023E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE1BBCD4-D0E0-4D01-8323-D4CFDF8E4F9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{5D1C55E5-96A3-4B43-BCBA-98C20E0AFC06}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{5D1C55E5-96A3-4B43-BCBA-98C20E0AFC06}"/>
   </bookViews>
   <sheets>
     <sheet name="Correlations" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="99">
   <si>
     <t xml:space="preserve">PRE-DIAGNOSTICS - CORRELATION TABLE FOR INDEPENDENT REGRESSION VARIABLES </t>
   </si>
@@ -448,6 +448,72 @@
   <si>
     <t xml:space="preserve">INDEPENDENT REGRESSION LIN LOG VARIABLES - PARAMETERS </t>
   </si>
+  <si>
+    <t>Lin Log  Elasticity Coeff</t>
+  </si>
+  <si>
+    <t>DW Watson Test</t>
+  </si>
+  <si>
+    <t>Autocorrelation</t>
+  </si>
+  <si>
+    <t>Statistic</t>
+  </si>
+  <si>
+    <t>P-value</t>
+  </si>
+  <si>
+    <t>Conclusion</t>
+  </si>
+  <si>
+    <t>Weak Negative AC</t>
+  </si>
+  <si>
+    <t>White Test</t>
+  </si>
+  <si>
+    <t>Errors are homoscedastic</t>
+  </si>
+  <si>
+    <t>INDEPENDENT LINEAR REGRESSION MODEL DIAGONISTICS</t>
+  </si>
+  <si>
+    <t>Shapiro Test</t>
+  </si>
+  <si>
+    <t>Errors distributed normally</t>
+  </si>
+  <si>
+    <t>Table 2.1</t>
+  </si>
+  <si>
+    <t>Plot 2.1: Actual Vs Fitted Values</t>
+  </si>
+  <si>
+    <t>Plot 2.2: Residual Over time</t>
+  </si>
+  <si>
+    <t>Plot 2.3: Residual QQ Plot</t>
+  </si>
+  <si>
+    <t>Plot 2.4: Histogram of Residuals</t>
+  </si>
+  <si>
+    <t>Plot 2.5: ACF Plot of Residuals</t>
+  </si>
+  <si>
+    <t>Plot 2.6: Residuals Vs Fitted Values</t>
+  </si>
+  <si>
+    <t>Plot 2.7: Scale Location Plot of Standardized Residuals</t>
+  </si>
+  <si>
+    <t>Plot 2.8: Cook's Distance Plot</t>
+  </si>
+  <si>
+    <t>Plot 2.9: Residual Vs Leverage Plot</t>
+  </si>
 </sst>
 </file>
 
@@ -460,7 +526,7 @@
     <numFmt numFmtId="167" formatCode="0.00000"/>
     <numFmt numFmtId="168" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -512,13 +578,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
@@ -619,7 +678,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -671,25 +730,46 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -707,6 +787,461 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>179410</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>90120</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D197442C-B26F-F313-B35D-50C030847ACA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="22972735"/>
+          <a:ext cx="7362825" cy="4863710"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>608859</xdr:colOff>
+      <xdr:row>140</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>561974</xdr:colOff>
+      <xdr:row>159</xdr:row>
+      <xdr:rowOff>17076</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{179FF809-BDE4-6A80-EC30-B7B769023B40}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="608859" y="28632151"/>
+          <a:ext cx="6372965" cy="3512750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>239</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>259</xdr:row>
+      <xdr:rowOff>103488</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0ACDB662-E804-E9A4-6881-0D032BB5DEE1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="638174" y="47463075"/>
+          <a:ext cx="6353176" cy="3818238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>264</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>573719</xdr:colOff>
+      <xdr:row>285</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7337D520-EA49-7650-0A34-9D2F46955860}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="619125" y="52187476"/>
+          <a:ext cx="6374444" cy="3943349"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3</xdr:colOff>
+      <xdr:row>289</xdr:row>
+      <xdr:rowOff>41103</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>310</xdr:row>
+      <xdr:rowOff>94533</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F00DBC99-EFAD-6724-B05B-0EE4B0C91D1F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609603" y="58267428"/>
+          <a:ext cx="6476997" cy="4053930"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>596518</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>105</xdr:row>
+      <xdr:rowOff>125326</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8184067-7A9E-793C-0F8C-FFEADCDA6BAD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="596518" y="16325851"/>
+          <a:ext cx="7404482" cy="5640300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>163</xdr:row>
+      <xdr:rowOff>26389</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>186</xdr:row>
+      <xdr:rowOff>182062</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F93F7A6-2689-7F12-198A-A690FF1DC815}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="561975" y="33106714"/>
+          <a:ext cx="6438900" cy="4537173"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>33291</xdr:colOff>
+      <xdr:row>191</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>210</xdr:row>
+      <xdr:rowOff>85238</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B65C81E9-C34D-660A-8C1C-69986A1250AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="642891" y="38242875"/>
+          <a:ext cx="6377034" cy="3685688"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>215</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>234</xdr:row>
+      <xdr:rowOff>180174</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Picture 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92E2D875-0342-8DB7-AC3C-37886F836AF7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="590550" y="42824400"/>
+          <a:ext cx="6400800" cy="3771099"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1028,8 +1563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13BEBFF8-48D8-4552-B3CF-92ECDE88DD45}">
   <dimension ref="B2:K20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1371,28 +1906,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53A1F66F-6B1A-47BA-B6E8-50FB1B5C3937}">
-  <dimension ref="B2:S69"/>
+  <dimension ref="B2:S288"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="I51" sqref="I51"/>
+    <sheetView topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J94" sqref="J94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.7109375" customWidth="1"/>
     <col min="11" max="11" width="24.7109375" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" customWidth="1"/>
-    <col min="14" max="15" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14" customWidth="1"/>
-    <col min="17" max="17" width="11.7109375" customWidth="1"/>
-    <col min="18" max="18" width="14" customWidth="1"/>
-    <col min="19" max="19" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="19" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1412,6 +1941,11 @@
         <v>25</v>
       </c>
     </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B4" s="22" t="s">
+        <v>89</v>
+      </c>
+    </row>
     <row r="5" spans="2:19" ht="30" x14ac:dyDescent="0.25">
       <c r="C5" s="11" t="s">
         <v>17</v>
@@ -1999,195 +2533,211 @@
       <c r="S16" s="4"/>
     </row>
     <row r="17" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="9"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="21"/>
-      <c r="M17" s="21"/>
-      <c r="N17" s="21"/>
-      <c r="O17" s="21"/>
-      <c r="P17" s="21"/>
-      <c r="Q17" s="21"/>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
+      <c r="B17" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="15">
+        <v>25260.869569999999</v>
+      </c>
+      <c r="D17" s="15">
+        <v>133.78</v>
+      </c>
+      <c r="E17" s="15">
+        <v>23.01</v>
+      </c>
+      <c r="F17" s="15">
+        <v>16.648929800000001</v>
+      </c>
+      <c r="G17" s="15">
+        <v>211561</v>
+      </c>
+      <c r="H17" s="15">
+        <v>45.750175400000003</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="L17" s="13">
+        <v>25260.869569999999</v>
+      </c>
+      <c r="M17" s="13">
+        <v>133.78</v>
+      </c>
+      <c r="N17" s="13">
+        <v>23.01</v>
+      </c>
+      <c r="O17" s="13">
+        <v>16.648929800000001</v>
+      </c>
+      <c r="P17" s="13">
+        <v>211561</v>
+      </c>
+      <c r="Q17" s="13">
+        <v>45.750175400000003</v>
+      </c>
+      <c r="R17" s="13">
+        <v>0.97050139999999996</v>
+      </c>
+      <c r="S17" s="13">
+        <v>0.37596190000000002</v>
+      </c>
     </row>
     <row r="18" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
+        <v>15</v>
+      </c>
+      <c r="C18" s="15">
+        <v>28627.372567070001</v>
+      </c>
+      <c r="D18" s="15">
+        <v>4.3487205800000002</v>
+      </c>
+      <c r="E18" s="15">
+        <v>0.67129057000000003</v>
+      </c>
+      <c r="F18" s="15">
+        <v>7.8548224500000003</v>
+      </c>
+      <c r="G18" s="15">
+        <v>441331.52875244</v>
+      </c>
+      <c r="H18" s="15">
+        <v>65.450477980000002</v>
+      </c>
       <c r="K18" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-    </row>
-    <row r="19" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="K19" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4"/>
-      <c r="Q19" s="4"/>
-      <c r="R19" s="4"/>
-      <c r="S19" s="4"/>
-    </row>
+        <v>15</v>
+      </c>
+      <c r="L18" s="13">
+        <v>28627.372567070001</v>
+      </c>
+      <c r="M18" s="13">
+        <v>4.3487205800000002</v>
+      </c>
+      <c r="N18" s="13">
+        <v>0.67129057000000003</v>
+      </c>
+      <c r="O18" s="13">
+        <v>7.8548224500000003</v>
+      </c>
+      <c r="P18" s="13">
+        <v>441331.52875244</v>
+      </c>
+      <c r="Q18" s="13">
+        <v>65.450477980000002</v>
+      </c>
+      <c r="R18" s="13">
+        <v>0.15834402</v>
+      </c>
+      <c r="S18" s="13">
+        <v>8.0331959999999994E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="15">
-        <v>25260.869569999999</v>
-      </c>
-      <c r="D20" s="15">
-        <v>133.78</v>
-      </c>
-      <c r="E20" s="15">
-        <v>23.01</v>
-      </c>
-      <c r="F20" s="15">
-        <v>16.648929800000001</v>
-      </c>
-      <c r="G20" s="15">
-        <v>211561</v>
-      </c>
-      <c r="H20" s="15">
-        <v>45.750175400000003</v>
-      </c>
-      <c r="K20" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="L20" s="13">
-        <v>25260.869569999999</v>
-      </c>
-      <c r="M20" s="13">
-        <v>133.78</v>
-      </c>
-      <c r="N20" s="13">
-        <v>23.01</v>
-      </c>
-      <c r="O20" s="13">
-        <v>16.648929800000001</v>
-      </c>
-      <c r="P20" s="13">
-        <v>211561</v>
-      </c>
-      <c r="Q20" s="13">
-        <v>45.750175400000003</v>
-      </c>
-      <c r="R20" s="13">
-        <v>0.97050139999999996</v>
-      </c>
-      <c r="S20" s="13">
-        <v>0.37596190000000002</v>
-      </c>
+      <c r="B20" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="41">
+        <v>0.89949999999999997</v>
+      </c>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
+      <c r="K20" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="L20" s="41">
+        <v>0.90529999999999999</v>
+      </c>
+      <c r="M20" s="41"/>
+      <c r="N20" s="41"/>
+      <c r="O20" s="41"/>
+      <c r="P20" s="41"/>
+      <c r="Q20" s="41"/>
+      <c r="R20" s="41"/>
+      <c r="S20" s="41"/>
     </row>
     <row r="21" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="15">
-        <v>28627.372567070001</v>
-      </c>
-      <c r="D21" s="15">
-        <v>4.3487205800000002</v>
-      </c>
-      <c r="E21" s="15">
-        <v>0.67129057000000003</v>
-      </c>
-      <c r="F21" s="15">
-        <v>7.8548224500000003</v>
-      </c>
-      <c r="G21" s="15">
-        <v>441331.52875244</v>
-      </c>
-      <c r="H21" s="15">
-        <v>65.450477980000002</v>
-      </c>
-      <c r="K21" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L21" s="13">
-        <v>28627.372567070001</v>
-      </c>
-      <c r="M21" s="13">
-        <v>4.3487205800000002</v>
-      </c>
-      <c r="N21" s="13">
-        <v>0.67129057000000003</v>
-      </c>
-      <c r="O21" s="13">
-        <v>7.8548224500000003</v>
-      </c>
-      <c r="P21" s="13">
-        <v>441331.52875244</v>
-      </c>
-      <c r="Q21" s="13">
-        <v>65.450477980000002</v>
-      </c>
-      <c r="R21" s="13">
-        <v>0.15834402</v>
-      </c>
-      <c r="S21" s="13">
-        <v>8.0331959999999994E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="E21" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="F21" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="40"/>
+      <c r="N21" s="40"/>
+      <c r="O21" s="40"/>
+      <c r="P21" s="40"/>
+      <c r="Q21" s="40"/>
+      <c r="R21" s="40"/>
+      <c r="S21" s="40"/>
+    </row>
+    <row r="22" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="35"/>
+      <c r="C22" s="35">
+        <v>-0.183</v>
+      </c>
+      <c r="D22" s="35">
+        <v>2.236059</v>
+      </c>
+      <c r="E22" s="35">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="F22" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
+    </row>
+    <row r="23" spans="2:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" s="27">
-        <v>0.89949999999999997</v>
-      </c>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
-      <c r="K23" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="L23" s="27">
-        <v>0.90529999999999999</v>
-      </c>
-      <c r="M23" s="27"/>
-      <c r="N23" s="27"/>
-      <c r="O23" s="27"/>
-      <c r="P23" s="27"/>
-      <c r="Q23" s="27"/>
-      <c r="R23" s="27"/>
-      <c r="S23" s="27"/>
-    </row>
-    <row r="24" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>84</v>
+      </c>
+      <c r="C23" s="35"/>
+      <c r="D23" s="36">
+        <v>3.9453</v>
+      </c>
+      <c r="E23" s="35">
+        <v>0.1391</v>
+      </c>
+      <c r="F23" s="38" t="s">
+        <v>85</v>
+      </c>
+      <c r="G23" s="35"/>
+      <c r="H23" s="35"/>
+    </row>
+    <row r="24" spans="2:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" s="35"/>
+      <c r="D24" s="36">
+        <v>0.98007</v>
+      </c>
+      <c r="E24" s="35">
+        <v>0.84</v>
+      </c>
+      <c r="F24" s="38" t="s">
+        <v>88</v>
+      </c>
+      <c r="G24" s="35"/>
+      <c r="H24" s="35"/>
+    </row>
     <row r="25" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="2:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="7" t="s">
@@ -2529,22 +3079,22 @@
       <c r="B36" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C36" s="13">
         <v>270.22919999999999</v>
       </c>
-      <c r="D36" s="4">
+      <c r="D36" s="13">
         <v>7.8691000000000004</v>
       </c>
-      <c r="E36" s="4">
+      <c r="E36" s="13">
         <v>11.508900000000001</v>
       </c>
-      <c r="F36" s="4">
+      <c r="F36" s="13">
         <v>26.261700000000001</v>
       </c>
-      <c r="G36" s="4">
+      <c r="G36" s="13">
         <v>9.3896999999999995</v>
       </c>
-      <c r="H36" s="4">
+      <c r="H36" s="13">
         <v>6.0850999999999997</v>
       </c>
       <c r="K36" s="9" t="s">
@@ -2579,22 +3129,22 @@
       <c r="B37" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C37" s="4">
+      <c r="C37" s="32">
         <v>7.6739999999999997E-14</v>
       </c>
-      <c r="D37" s="4">
+      <c r="D37" s="32">
         <v>1.0312999999999999E-2</v>
       </c>
-      <c r="E37" s="4">
+      <c r="E37" s="32">
         <v>2.6180000000000001E-3</v>
       </c>
-      <c r="F37" s="4">
+      <c r="F37" s="32">
         <v>3.898100251792E-5</v>
       </c>
-      <c r="G37" s="4">
+      <c r="G37" s="32">
         <v>5.6800000000000002E-3</v>
       </c>
-      <c r="H37" s="4">
+      <c r="H37" s="32">
         <v>2.1895000000000001E-2</v>
       </c>
       <c r="K37" s="9" t="s">
@@ -2606,10 +3156,10 @@
       <c r="M37" s="13">
         <v>1.4213E-2</v>
       </c>
-      <c r="N37" s="13">
+      <c r="N37" s="33">
         <v>4.0280000000000003E-3</v>
       </c>
-      <c r="O37" s="13">
+      <c r="O37" s="32">
         <v>8.52378452475E-5</v>
       </c>
       <c r="P37" s="13">
@@ -2880,27 +3430,27 @@
       <c r="B45" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C45" s="27">
+      <c r="C45" s="41">
         <v>0.93769999999999998</v>
       </c>
-      <c r="D45" s="27"/>
-      <c r="E45" s="27"/>
-      <c r="F45" s="27"/>
-      <c r="G45" s="27"/>
-      <c r="H45" s="27"/>
+      <c r="D45" s="41"/>
+      <c r="E45" s="41"/>
+      <c r="F45" s="41"/>
+      <c r="G45" s="41"/>
+      <c r="H45" s="41"/>
       <c r="K45" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="L45" s="27">
+      <c r="L45" s="41">
         <v>0.93830000000000002</v>
       </c>
-      <c r="M45" s="27"/>
-      <c r="N45" s="27"/>
-      <c r="O45" s="27"/>
-      <c r="P45" s="27"/>
-      <c r="Q45" s="27"/>
-      <c r="R45" s="27"/>
-      <c r="S45" s="27"/>
+      <c r="M45" s="41"/>
+      <c r="N45" s="41"/>
+      <c r="O45" s="41"/>
+      <c r="P45" s="41"/>
+      <c r="Q45" s="41"/>
+      <c r="R45" s="41"/>
+      <c r="S45" s="41"/>
     </row>
     <row r="50" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B50" s="7" t="s">
@@ -3008,102 +3558,220 @@
     </row>
     <row r="55" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B55" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C55" s="13"/>
-      <c r="D55" s="13"/>
-      <c r="E55" s="13"/>
-      <c r="F55" s="13"/>
-      <c r="G55" s="13"/>
-      <c r="H55" s="13"/>
+        <v>77</v>
+      </c>
+      <c r="C55" s="13">
+        <v>-618.79999999999995</v>
+      </c>
+      <c r="D55" s="13">
+        <v>-858.1</v>
+      </c>
+      <c r="E55" s="13">
+        <v>586.20000000000005</v>
+      </c>
+      <c r="F55" s="13">
+        <v>732.3</v>
+      </c>
+      <c r="G55" s="13">
+        <v>114.2</v>
+      </c>
+      <c r="H55" s="13">
+        <v>496.7</v>
+      </c>
       <c r="K55" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="L55" s="13"/>
-      <c r="M55" s="13"/>
-      <c r="N55" s="13"/>
-      <c r="O55" s="13"/>
-      <c r="P55" s="13"/>
-      <c r="Q55" s="13"/>
-      <c r="R55" s="13"/>
-      <c r="S55" s="24"/>
+        <v>77</v>
+      </c>
+      <c r="L55" s="13">
+        <v>-398</v>
+      </c>
+      <c r="M55" s="13">
+        <v>-435.8</v>
+      </c>
+      <c r="N55" s="13">
+        <v>-166.4</v>
+      </c>
+      <c r="O55" s="13">
+        <v>689.5</v>
+      </c>
+      <c r="P55" s="13">
+        <v>133.5</v>
+      </c>
+      <c r="Q55" s="13">
+        <v>337.8</v>
+      </c>
+      <c r="R55" s="13">
+        <v>213.5</v>
+      </c>
+      <c r="S55" s="24">
+        <v>-133.19999999999999</v>
+      </c>
     </row>
     <row r="56" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B56" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C56" s="13"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="13"/>
-      <c r="F56" s="13"/>
-      <c r="G56" s="13"/>
-      <c r="H56" s="13"/>
+      <c r="C56" s="13">
+        <v>-2.9079999999999999</v>
+      </c>
+      <c r="D56" s="13">
+        <v>-0.63600000000000001</v>
+      </c>
+      <c r="E56" s="13">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="F56" s="13">
+        <v>1.73</v>
+      </c>
+      <c r="G56" s="13">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="H56" s="13">
+        <v>2.2890000000000001</v>
+      </c>
       <c r="K56" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="L56" s="13"/>
-      <c r="M56" s="13"/>
-      <c r="N56" s="13"/>
-      <c r="O56" s="13"/>
-      <c r="P56" s="13"/>
-      <c r="Q56" s="13"/>
-      <c r="R56" s="13"/>
-      <c r="S56" s="24"/>
+      <c r="L56" s="13">
+        <v>-1.054</v>
+      </c>
+      <c r="M56" s="13">
+        <v>-0.223</v>
+      </c>
+      <c r="N56" s="13">
+        <v>-7.3999999999999996E-2</v>
+      </c>
+      <c r="O56" s="13">
+        <v>1.5389999999999999</v>
+      </c>
+      <c r="P56" s="13">
+        <v>0.69199999999999995</v>
+      </c>
+      <c r="Q56" s="13">
+        <v>1.1910000000000001</v>
+      </c>
+      <c r="R56" s="13">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="S56" s="24">
+        <v>-0.51900000000000002</v>
+      </c>
     </row>
     <row r="57" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B57" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C57" s="13"/>
-      <c r="D57" s="13"/>
-      <c r="E57" s="13"/>
-      <c r="F57" s="13"/>
-      <c r="G57" s="13"/>
-      <c r="H57" s="13"/>
+      <c r="C57" s="13">
+        <v>8.1499999999999993E-3</v>
+      </c>
+      <c r="D57" s="13">
+        <v>0.53141000000000005</v>
+      </c>
+      <c r="E57" s="13">
+        <v>0.7702</v>
+      </c>
+      <c r="F57" s="13">
+        <v>9.7570000000000004E-2</v>
+      </c>
+      <c r="G57" s="13">
+        <v>0.4758</v>
+      </c>
+      <c r="H57" s="13">
+        <v>3.2050000000000002E-2</v>
+      </c>
       <c r="K57" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="L57" s="13"/>
-      <c r="M57" s="13"/>
-      <c r="N57" s="13"/>
-      <c r="O57" s="13"/>
-      <c r="P57" s="13"/>
-      <c r="Q57" s="13"/>
-      <c r="R57" s="13"/>
-      <c r="S57" s="24"/>
+      <c r="L57" s="13">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="M57" s="13">
+        <v>0.82599999999999996</v>
+      </c>
+      <c r="N57" s="13">
+        <v>0.94199999999999995</v>
+      </c>
+      <c r="O57" s="13">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="P57" s="13">
+        <v>0.497</v>
+      </c>
+      <c r="Q57" s="13">
+        <v>0.248</v>
+      </c>
+      <c r="R57" s="13">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="S57" s="24">
+        <v>0.61</v>
+      </c>
     </row>
     <row r="58" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B58" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C58" s="18"/>
-      <c r="D58" s="19"/>
-      <c r="E58" s="19"/>
-      <c r="F58" s="20"/>
-      <c r="G58" s="19"/>
-      <c r="H58" s="20"/>
+      <c r="C58" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D58" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E58" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="F58" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="G58" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="H58" s="18" t="s">
+        <v>33</v>
+      </c>
       <c r="K58" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="L58" s="18"/>
-      <c r="M58" s="19"/>
-      <c r="N58" s="19"/>
-      <c r="O58" s="19"/>
-      <c r="P58" s="19"/>
-      <c r="Q58" s="18"/>
-      <c r="R58" s="19"/>
-      <c r="S58" s="19"/>
+      <c r="L58" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="M58" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="N58" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="O58" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="P58" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q58" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="R58" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="S58" s="19" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="59" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B59" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C59" s="21"/>
+      <c r="C59" s="21">
+        <v>0.99</v>
+      </c>
       <c r="D59" s="21"/>
       <c r="E59" s="21"/>
-      <c r="F59" s="21"/>
+      <c r="F59" s="21">
+        <v>0.9</v>
+      </c>
       <c r="G59" s="21"/>
-      <c r="H59" s="21"/>
+      <c r="H59" s="21">
+        <v>0.95</v>
+      </c>
       <c r="K59" s="9" t="s">
         <v>36</v>
       </c>
@@ -3120,87 +3788,191 @@
       <c r="B60" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C60" s="4"/>
-      <c r="D60" s="4"/>
-      <c r="E60" s="4"/>
-      <c r="F60" s="4"/>
-      <c r="G60" s="4"/>
-      <c r="H60" s="4"/>
+      <c r="C60" s="13">
+        <v>237.51759999999999</v>
+      </c>
+      <c r="D60" s="13">
+        <v>2.3288000000000002</v>
+      </c>
+      <c r="E60" s="13">
+        <v>9.8490000000000002</v>
+      </c>
+      <c r="F60" s="13">
+        <v>24.9954</v>
+      </c>
+      <c r="G60" s="13">
+        <v>10.149100000000001</v>
+      </c>
+      <c r="H60" s="13">
+        <v>5.2389999999999999</v>
+      </c>
       <c r="K60" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L60" s="13"/>
-      <c r="M60" s="13"/>
-      <c r="N60" s="13"/>
-      <c r="O60" s="13"/>
-      <c r="P60" s="13"/>
-      <c r="Q60" s="13"/>
-      <c r="R60" s="13"/>
-      <c r="S60" s="13"/>
+      <c r="L60" s="13">
+        <v>224.91569999999999</v>
+      </c>
+      <c r="M60" s="13">
+        <v>2.2052999999999998</v>
+      </c>
+      <c r="N60" s="13">
+        <v>9.3264999999999993</v>
+      </c>
+      <c r="O60" s="13">
+        <v>23.6693</v>
+      </c>
+      <c r="P60" s="13">
+        <v>9.6105999999999998</v>
+      </c>
+      <c r="Q60" s="13">
+        <v>4.9610000000000003</v>
+      </c>
+      <c r="R60" s="13">
+        <v>0.56369999999999998</v>
+      </c>
+      <c r="S60" s="13">
+        <v>0.26910000000000001</v>
+      </c>
     </row>
     <row r="61" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B61" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C61" s="4"/>
-      <c r="D61" s="4"/>
-      <c r="E61" s="4"/>
-      <c r="F61" s="4"/>
-      <c r="G61" s="4"/>
-      <c r="H61" s="4"/>
+      <c r="C61" s="4">
+        <v>2.8460000000000002E-13</v>
+      </c>
+      <c r="D61" s="13">
+        <v>0.14124500000000001</v>
+      </c>
+      <c r="E61" s="33">
+        <v>4.777E-3</v>
+      </c>
+      <c r="F61" s="32">
+        <v>5.27423231349E-5</v>
+      </c>
+      <c r="G61" s="33">
+        <v>4.2729999999999999E-3</v>
+      </c>
+      <c r="H61" s="12">
+        <v>3.2052999999999998E-2</v>
+      </c>
       <c r="K61" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L61" s="13"/>
-      <c r="M61" s="13"/>
-      <c r="N61" s="13"/>
-      <c r="O61" s="13"/>
-      <c r="P61" s="13"/>
-      <c r="Q61" s="13"/>
-      <c r="R61" s="13"/>
-      <c r="S61" s="13"/>
+      <c r="L61" s="4">
+        <v>2.4150000000000001E-12</v>
+      </c>
+      <c r="M61" s="13">
+        <v>0.15312999999999999</v>
+      </c>
+      <c r="N61" s="13">
+        <v>6.2659999999999999E-3</v>
+      </c>
+      <c r="O61" s="32">
+        <v>9.3779385808000006E-5</v>
+      </c>
+      <c r="P61" s="13">
+        <v>5.6439999999999997E-3</v>
+      </c>
+      <c r="Q61" s="13">
+        <v>3.7571E-2</v>
+      </c>
+      <c r="R61" s="13">
+        <v>0.46152100000000001</v>
+      </c>
+      <c r="S61" s="13">
+        <v>0.60964799999999997</v>
+      </c>
     </row>
     <row r="62" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B62" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C62" s="18"/>
-      <c r="D62" s="18"/>
-      <c r="E62" s="18"/>
-      <c r="F62" s="18"/>
-      <c r="G62" s="18"/>
-      <c r="H62" s="18"/>
+      <c r="C62" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D62" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E62" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F62" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="G62" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="H62" s="18" t="s">
+        <v>33</v>
+      </c>
       <c r="K62" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="L62" s="18"/>
-      <c r="M62" s="18"/>
-      <c r="N62" s="18"/>
-      <c r="O62" s="18"/>
-      <c r="P62" s="18"/>
-      <c r="Q62" s="18"/>
-      <c r="R62" s="19"/>
-      <c r="S62" s="19"/>
+      <c r="L62" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M62" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="N62" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="O62" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="P62" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q62" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="R62" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="S62" s="19" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="63" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B63" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C63" s="21"/>
+      <c r="C63" s="21">
+        <v>0.99</v>
+      </c>
       <c r="D63" s="21"/>
-      <c r="E63" s="21"/>
-      <c r="F63" s="21"/>
-      <c r="G63" s="21"/>
-      <c r="H63" s="21"/>
+      <c r="E63" s="21">
+        <v>0.99</v>
+      </c>
+      <c r="F63" s="21">
+        <v>0.99</v>
+      </c>
+      <c r="G63" s="21">
+        <v>0.99</v>
+      </c>
+      <c r="H63" s="21">
+        <v>0.95</v>
+      </c>
       <c r="K63" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="L63" s="21"/>
+      <c r="L63" s="21">
+        <v>0.99</v>
+      </c>
       <c r="M63" s="21"/>
-      <c r="N63" s="21"/>
-      <c r="O63" s="21"/>
-      <c r="P63" s="21"/>
-      <c r="Q63" s="21"/>
+      <c r="N63" s="21">
+        <v>0.99</v>
+      </c>
+      <c r="O63" s="21">
+        <v>0.99</v>
+      </c>
+      <c r="P63" s="21">
+        <v>0.99</v>
+      </c>
+      <c r="Q63" s="21">
+        <v>0.95</v>
+      </c>
       <c r="R63" s="4"/>
       <c r="S63" s="4"/>
     </row>
@@ -3252,45 +4024,101 @@
       <c r="B66" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C66" s="13"/>
-      <c r="D66" s="13"/>
-      <c r="E66" s="13"/>
-      <c r="F66" s="13"/>
-      <c r="G66" s="13"/>
-      <c r="H66" s="13"/>
+      <c r="C66" s="13">
+        <v>10.1370118</v>
+      </c>
+      <c r="D66" s="13">
+        <v>4.8961967</v>
+      </c>
+      <c r="E66" s="13">
+        <v>3.1359289000000001</v>
+      </c>
+      <c r="F66" s="13">
+        <v>2.8123459</v>
+      </c>
+      <c r="G66" s="13">
+        <v>12.2622687</v>
+      </c>
+      <c r="H66" s="13">
+        <v>3.8231956</v>
+      </c>
       <c r="K66" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="L66" s="13"/>
-      <c r="M66" s="13"/>
-      <c r="N66" s="13"/>
-      <c r="O66" s="13"/>
-      <c r="P66" s="13"/>
-      <c r="Q66" s="13"/>
-      <c r="R66" s="13"/>
-      <c r="S66" s="13"/>
+      <c r="L66" s="13">
+        <v>10.1370118</v>
+      </c>
+      <c r="M66" s="13">
+        <v>4.8961967</v>
+      </c>
+      <c r="N66" s="13">
+        <v>3.1359289000000001</v>
+      </c>
+      <c r="O66" s="13">
+        <v>2.8123459</v>
+      </c>
+      <c r="P66" s="13">
+        <v>12.2622687</v>
+      </c>
+      <c r="Q66" s="13">
+        <v>3.8231956</v>
+      </c>
+      <c r="R66" s="13">
+        <v>-2.9942400000000001E-2</v>
+      </c>
+      <c r="S66" s="13">
+        <v>-0.97826749999999996</v>
+      </c>
     </row>
     <row r="67" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B67" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C67" s="13"/>
-      <c r="D67" s="13"/>
-      <c r="E67" s="13"/>
-      <c r="F67" s="13"/>
-      <c r="G67" s="13"/>
-      <c r="H67" s="13"/>
+      <c r="C67" s="13">
+        <v>0.76928872999999998</v>
+      </c>
+      <c r="D67" s="13">
+        <v>3.2674689999999999E-2</v>
+      </c>
+      <c r="E67" s="13">
+        <v>2.9203030000000001E-2</v>
+      </c>
+      <c r="F67" s="13">
+        <v>0.48294925999999999</v>
+      </c>
+      <c r="G67" s="13">
+        <v>1.4311327</v>
+      </c>
+      <c r="H67" s="13">
+        <v>1.0960862899999999</v>
+      </c>
       <c r="K67" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="L67" s="13"/>
-      <c r="M67" s="13"/>
-      <c r="N67" s="13"/>
-      <c r="O67" s="13"/>
-      <c r="P67" s="13"/>
-      <c r="Q67" s="13"/>
-      <c r="R67" s="13"/>
-      <c r="S67" s="13"/>
+      <c r="L67" s="13">
+        <v>0.76928872999999998</v>
+      </c>
+      <c r="M67" s="13">
+        <v>3.2674689999999999E-2</v>
+      </c>
+      <c r="N67" s="13">
+        <v>2.9203030000000001E-2</v>
+      </c>
+      <c r="O67" s="13">
+        <v>0.48294925999999999</v>
+      </c>
+      <c r="P67" s="13">
+        <v>1.4311327</v>
+      </c>
+      <c r="Q67" s="13">
+        <v>1.0960862899999999</v>
+      </c>
+      <c r="R67" s="13">
+        <v>0.17738045</v>
+      </c>
+      <c r="S67" s="13">
+        <v>0.26867327000000002</v>
+      </c>
     </row>
     <row r="68" spans="2:19" x14ac:dyDescent="0.25">
       <c r="K68" s="22"/>
@@ -3307,38 +4135,94 @@
       <c r="B69" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C69" s="27">
-        <v>0.93769999999999998</v>
-      </c>
-      <c r="D69" s="27"/>
-      <c r="E69" s="27"/>
-      <c r="F69" s="27"/>
-      <c r="G69" s="27"/>
-      <c r="H69" s="27"/>
+      <c r="C69" s="41">
+        <v>0.92949999999999999</v>
+      </c>
+      <c r="D69" s="41"/>
+      <c r="E69" s="41"/>
+      <c r="F69" s="41"/>
+      <c r="G69" s="41"/>
+      <c r="H69" s="41"/>
       <c r="K69" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="L69" s="27">
-        <v>0.93830000000000002</v>
-      </c>
-      <c r="M69" s="27"/>
-      <c r="N69" s="27"/>
-      <c r="O69" s="27"/>
-      <c r="P69" s="27"/>
-      <c r="Q69" s="27"/>
-      <c r="R69" s="27"/>
-      <c r="S69" s="27"/>
+      <c r="L69" s="41"/>
+      <c r="M69" s="41"/>
+      <c r="N69" s="41"/>
+      <c r="O69" s="41"/>
+      <c r="P69" s="41"/>
+      <c r="Q69" s="41"/>
+      <c r="R69" s="41"/>
+      <c r="S69" s="41"/>
+    </row>
+    <row r="72" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B72" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="73" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B73" s="7"/>
+    </row>
+    <row r="75" spans="2:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="B75" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B109" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B139" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="162" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B162" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="190" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B190" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="213" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B213" s="22"/>
+    </row>
+    <row r="214" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B214" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="238" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B238" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="263" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B263" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="288" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B288" s="11" t="s">
+        <v>98</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="C23:H23"/>
-    <mergeCell ref="L23:S23"/>
+    <mergeCell ref="C20:H20"/>
+    <mergeCell ref="L20:S20"/>
     <mergeCell ref="C45:H45"/>
     <mergeCell ref="L45:S45"/>
     <mergeCell ref="C69:H69"/>
     <mergeCell ref="L69:S69"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3346,8 +4230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91BE7346-DFF9-4F39-8295-2A32804F99B3}">
   <dimension ref="B2:J25"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3361,12 +4245,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="30" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="2:10" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="28"/>
+    <row r="3" spans="2:10" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="27"/>
       <c r="C3" s="11" t="s">
         <v>17</v>
       </c>
@@ -3392,245 +4276,245 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="2:10" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="29">
+      <c r="C4" s="28">
         <v>1</v>
       </c>
-      <c r="D4" s="30">
+      <c r="D4" s="29">
         <v>43335116.93</v>
       </c>
-      <c r="E4" s="30">
+      <c r="E4" s="29">
         <v>1818619663.0599999</v>
       </c>
-      <c r="F4" s="30">
+      <c r="F4" s="29">
         <v>12441767.369999999</v>
       </c>
-      <c r="G4" s="29">
+      <c r="G4" s="28">
         <v>0</v>
       </c>
-      <c r="H4" s="30">
+      <c r="H4" s="29">
         <v>191309.85</v>
       </c>
-      <c r="I4" s="30">
+      <c r="I4" s="29">
         <v>32685839312.189999</v>
       </c>
-      <c r="J4" s="30">
+      <c r="J4" s="29">
         <v>126994887993.28</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="29">
+      <c r="C5" s="28">
         <v>0</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5" s="28">
         <v>1</v>
       </c>
-      <c r="E5" s="29">
+      <c r="E5" s="28">
         <v>41.97</v>
       </c>
-      <c r="F5" s="29">
+      <c r="F5" s="28">
         <v>0.28999999999999998</v>
       </c>
-      <c r="G5" s="29">
+      <c r="G5" s="28">
         <v>0</v>
       </c>
-      <c r="H5" s="29">
+      <c r="H5" s="28">
         <v>0</v>
       </c>
-      <c r="I5" s="29">
+      <c r="I5" s="28">
         <v>754.26</v>
       </c>
-      <c r="J5" s="30">
+      <c r="J5" s="29">
         <v>2930.53</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="29">
+      <c r="C6" s="28">
         <v>0</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6" s="28">
         <v>0.02</v>
       </c>
-      <c r="E6" s="29">
+      <c r="E6" s="28">
         <v>1</v>
       </c>
-      <c r="F6" s="29">
+      <c r="F6" s="28">
         <v>0.01</v>
       </c>
-      <c r="G6" s="29">
+      <c r="G6" s="28">
         <v>0</v>
       </c>
-      <c r="H6" s="29">
+      <c r="H6" s="28">
         <v>0</v>
       </c>
-      <c r="I6" s="29">
+      <c r="I6" s="28">
         <v>17.97</v>
       </c>
-      <c r="J6" s="29">
+      <c r="J6" s="28">
         <v>69.83</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="29">
+      <c r="C7" s="28">
         <v>0</v>
       </c>
-      <c r="D7" s="29">
+      <c r="D7" s="28">
         <v>3.48</v>
       </c>
-      <c r="E7" s="29">
+      <c r="E7" s="28">
         <v>146.16999999999999</v>
       </c>
-      <c r="F7" s="29">
+      <c r="F7" s="28">
         <v>1</v>
       </c>
-      <c r="G7" s="29">
+      <c r="G7" s="28">
         <v>0</v>
       </c>
-      <c r="H7" s="29">
+      <c r="H7" s="28">
         <v>0.02</v>
       </c>
-      <c r="I7" s="30">
+      <c r="I7" s="29">
         <v>2627.11</v>
       </c>
-      <c r="J7" s="30">
+      <c r="J7" s="29">
         <v>10207.14</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="29">
+      <c r="C8" s="28">
         <v>237.67</v>
       </c>
-      <c r="D8" s="30">
+      <c r="D8" s="29">
         <v>10299280864.790001</v>
       </c>
-      <c r="E8" s="30">
+      <c r="E8" s="29">
         <v>432223933477.03998</v>
       </c>
-      <c r="F8" s="30">
+      <c r="F8" s="29">
         <v>2956984211.5300002</v>
       </c>
-      <c r="G8" s="29">
+      <c r="G8" s="28">
         <v>1</v>
       </c>
-      <c r="H8" s="30">
+      <c r="H8" s="29">
         <v>45467833.829999998</v>
       </c>
-      <c r="I8" s="30">
+      <c r="I8" s="29">
         <v>7768310396890.7803</v>
       </c>
-      <c r="J8" s="30">
+      <c r="J8" s="29">
         <v>30182358156010.5</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="29">
+      <c r="C9" s="28">
         <v>0</v>
       </c>
-      <c r="D9" s="29">
+      <c r="D9" s="28">
         <v>226.52</v>
       </c>
-      <c r="E9" s="30">
+      <c r="E9" s="29">
         <v>9506.15</v>
       </c>
-      <c r="F9" s="29">
+      <c r="F9" s="28">
         <v>65.03</v>
       </c>
-      <c r="G9" s="29">
+      <c r="G9" s="28">
         <v>0</v>
       </c>
-      <c r="H9" s="29">
+      <c r="H9" s="28">
         <v>1</v>
       </c>
-      <c r="I9" s="30">
+      <c r="I9" s="29">
         <v>170852.88</v>
       </c>
-      <c r="J9" s="30">
+      <c r="J9" s="29">
         <v>663817.81999999995</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="29">
+      <c r="C10" s="28">
         <v>0</v>
       </c>
-      <c r="D10" s="29">
+      <c r="D10" s="28">
         <v>0</v>
       </c>
-      <c r="E10" s="29">
+      <c r="E10" s="28">
         <v>0.06</v>
       </c>
-      <c r="F10" s="29">
+      <c r="F10" s="28">
         <v>0</v>
       </c>
-      <c r="G10" s="29">
+      <c r="G10" s="28">
         <v>0</v>
       </c>
-      <c r="H10" s="29">
+      <c r="H10" s="28">
         <v>0</v>
       </c>
-      <c r="I10" s="29">
+      <c r="I10" s="28">
         <v>1</v>
       </c>
-      <c r="J10" s="29">
+      <c r="J10" s="28">
         <v>3.89</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="29">
+      <c r="C11" s="28">
         <v>0</v>
       </c>
-      <c r="D11" s="29">
+      <c r="D11" s="28">
         <v>0</v>
       </c>
-      <c r="E11" s="29">
+      <c r="E11" s="28">
         <v>0.01</v>
       </c>
-      <c r="F11" s="29">
+      <c r="F11" s="28">
         <v>0</v>
       </c>
-      <c r="G11" s="29">
+      <c r="G11" s="28">
         <v>0</v>
       </c>
-      <c r="H11" s="29">
+      <c r="H11" s="28">
         <v>0</v>
       </c>
-      <c r="I11" s="29">
+      <c r="I11" s="28">
         <v>0.26</v>
       </c>
-      <c r="J11" s="29">
+      <c r="J11" s="28">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="30" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="32"/>
+      <c r="B17" s="31"/>
       <c r="C17" s="11" t="s">
         <v>17</v>
       </c>
@@ -3656,235 +4540,235 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:10" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="C18" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="33" t="s">
+      <c r="D18" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="E18" s="33" t="s">
+      <c r="E18" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="33" t="s">
+      <c r="F18" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="G18" s="33" t="s">
+      <c r="G18" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="H18" s="33" t="s">
+      <c r="H18" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="I18" s="33" t="s">
+      <c r="I18" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="J18" s="33" t="s">
+      <c r="J18" s="42" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="2:10" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="33" t="s">
+      <c r="D19" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="E19" s="33" t="s">
+      <c r="E19" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="F19" s="33" t="s">
+      <c r="F19" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="G19" s="33" t="s">
+      <c r="G19" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="H19" s="33" t="s">
+      <c r="H19" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="I19" s="33" t="s">
+      <c r="I19" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="J19" s="33" t="s">
+      <c r="J19" s="42" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="2:10" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="33" t="s">
+      <c r="C20" s="42" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="33" t="s">
+      <c r="D20" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="33" t="s">
+      <c r="E20" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="F20" s="33" t="s">
+      <c r="F20" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="G20" s="33" t="s">
+      <c r="G20" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="H20" s="33" t="s">
+      <c r="H20" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="I20" s="33" t="s">
+      <c r="I20" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="J20" s="33" t="s">
+      <c r="J20" s="42" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="2:10" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="33" t="s">
+      <c r="C21" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="33" t="s">
+      <c r="D21" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="E21" s="33" t="s">
+      <c r="E21" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="F21" s="33" t="s">
+      <c r="F21" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="G21" s="33" t="s">
+      <c r="G21" s="42" t="s">
         <v>57</v>
       </c>
-      <c r="H21" s="33" t="s">
+      <c r="H21" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="I21" s="33" t="s">
+      <c r="I21" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="33" t="s">
+      <c r="J21" s="42" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="2:10" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="33" t="s">
+      <c r="C22" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="33" t="s">
+      <c r="D22" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="33" t="s">
+      <c r="E22" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="F22" s="33" t="s">
+      <c r="F22" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="G22" s="33" t="s">
+      <c r="G22" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="H22" s="33" t="s">
+      <c r="H22" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="I22" s="33" t="s">
+      <c r="I22" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="J22" s="33" t="s">
+      <c r="J22" s="42" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="2:10" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="33" t="s">
+      <c r="C23" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="D23" s="33" t="s">
+      <c r="D23" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="E23" s="33" t="s">
+      <c r="E23" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="F23" s="33" t="s">
+      <c r="F23" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="G23" s="33" t="s">
+      <c r="G23" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="H23" s="33" t="s">
+      <c r="H23" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="I23" s="33" t="s">
+      <c r="I23" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="J23" s="33" t="s">
+      <c r="J23" s="42" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="2:10" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="33" t="s">
+      <c r="C24" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="D24" s="33" t="s">
+      <c r="D24" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="E24" s="33" t="s">
+      <c r="E24" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="F24" s="33" t="s">
+      <c r="F24" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="G24" s="33" t="s">
+      <c r="G24" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="H24" s="33" t="s">
+      <c r="H24" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="I24" s="33" t="s">
+      <c r="I24" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="J24" s="33" t="s">
+      <c r="J24" s="42" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="2:10" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="33" t="s">
+      <c r="C25" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="D25" s="33" t="s">
+      <c r="D25" s="42" t="s">
         <v>69</v>
       </c>
-      <c r="E25" s="33" t="s">
+      <c r="E25" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="F25" s="33" t="s">
+      <c r="F25" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="G25" s="33" t="s">
+      <c r="G25" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="H25" s="33" t="s">
+      <c r="H25" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="I25" s="33" t="s">
+      <c r="I25" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="J25" s="33" t="s">
+      <c r="J25" s="42" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>